<commit_message>
foi alterado o documento com um espaço
</commit_message>
<xml_diff>
--- a/Gerencia de Requisitos/Definicoes de Sistema/THEMAG_CONDOC_Planilha de casos de uso.xlsx
+++ b/Gerencia de Requisitos/Definicoes de Sistema/THEMAG_CONDOC_Planilha de casos de uso.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="15195" windowHeight="8190" tabRatio="610" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="12" windowWidth="15192" windowHeight="8196" tabRatio="610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Posicionamento - Entrega 01" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="109">
   <si>
     <t>Módulo</t>
   </si>
@@ -341,13 +341,16 @@
   </si>
   <si>
     <t>UC003 - Manter Distrato de Contratos e Convenios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC004 - Detalhar Execucão </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,6 +653,79 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -659,6 +735,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -668,138 +750,59 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,6 +812,11 @@
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela Dinâmica 1" table="0" count="0"/>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -887,6 +895,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -921,6 +930,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1096,42 +1106,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.5703125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="77.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" style="2"/>
-    <col min="2" max="2" width="68.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="59.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="77.5703125" style="2"/>
+    <col min="1" max="1" width="77.5546875" style="2"/>
+    <col min="2" max="2" width="68.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="59.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="54.5546875" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="77.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="29" t="s">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" ht="15">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1148,151 +1158,151 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12.75" customHeight="1">
-      <c r="A4" s="37" t="s">
+    <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="35" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="42" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="32"/>
-    </row>
-    <row r="6" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="32"/>
-    </row>
-    <row r="7" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A7" s="38"/>
-      <c r="B7" s="41"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1">
-      <c r="A8" s="38"/>
-      <c r="B8" s="41"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="38"/>
-      <c r="B9" s="42" t="s">
+      <c r="D8" s="43"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="50" t="s">
         <v>106</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="E9" s="44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="11.25" customHeight="1">
-      <c r="A10" s="38"/>
-      <c r="B10" s="43"/>
+    <row r="10" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="35"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A11" s="38"/>
-      <c r="B11" s="43"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="45"/>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="35"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A12" s="38"/>
-      <c r="B12" s="43"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="45"/>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A13" s="38"/>
-      <c r="B13" s="40" t="s">
+      <c r="D12" s="49"/>
+      <c r="E12" s="46"/>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="35" t="s">
         <v>107</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A14" s="38"/>
-      <c r="B14" s="41"/>
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="45"/>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="41"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="45"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A16" s="39"/>
-      <c r="B16" s="69"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="46"/>
-    </row>
-    <row r="17" spans="5:5">
+      <c r="D16" s="54"/>
+      <c r="E16" s="34"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="5:5">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
     </row>
   </sheetData>
@@ -1316,520 +1326,504 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:E35"/>
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="20.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="73.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="20.85546875" style="2"/>
+    <col min="1" max="1" width="58.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="73.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="20.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="29" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-    </row>
-    <row r="3" spans="1:5" ht="11.25" customHeight="1">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
+    </row>
+    <row r="3" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="52" t="s">
-        <v>56</v>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>108</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="52"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
       <c r="B5" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="53"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="59"/>
       <c r="B6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="51" t="s">
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A8" s="52"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
       <c r="B8" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A9" s="52"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
       <c r="B9" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A10" s="52"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
       <c r="B10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-    </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A11" s="52"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+    </row>
+    <row r="11" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
       <c r="B11" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-    </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A12" s="53"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+    </row>
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
       <c r="B12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-    </row>
-    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A13" s="52" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+    </row>
+    <row r="13" spans="1:5" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-    </row>
-    <row r="14" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A14" s="52"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+    </row>
+    <row r="14" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
       <c r="B14" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A15" s="52"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+    </row>
+    <row r="15" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
       <c r="B15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-    </row>
-    <row r="16" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A16" s="52"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+    </row>
+    <row r="16" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
       <c r="B16" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-    </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A17" s="52"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
       <c r="B17" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A18" s="52"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
       <c r="B18" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A19" s="52"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
       <c r="B19" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A20" s="53"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+    </row>
+    <row r="20" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
       <c r="B20" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="71"/>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A21" s="51" t="s">
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+    </row>
+    <row r="21" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="57" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-    </row>
-    <row r="22" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A22" s="52"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
       <c r="B22" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A23" s="52"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+    </row>
+    <row r="23" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
       <c r="B23" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-    </row>
-    <row r="24" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A24" s="52"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+    </row>
+    <row r="24" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
       <c r="B24" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-    </row>
-    <row r="25" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A25" s="52"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+    </row>
+    <row r="25" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
       <c r="B25" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-    </row>
-    <row r="26" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A26" s="52"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+    </row>
+    <row r="26" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
       <c r="B26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-    </row>
-    <row r="27" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A27" s="52"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="55"/>
+    </row>
+    <row r="27" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="58"/>
       <c r="B27" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-    </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A28" s="52"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+    </row>
+    <row r="28" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
       <c r="B28" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A29" s="53"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+    </row>
+    <row r="29" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
       <c r="B29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-    </row>
-    <row r="30" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A30" s="51" t="s">
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+    </row>
+    <row r="30" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="57" t="s">
         <v>65</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-    </row>
-    <row r="31" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A31" s="52"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+    </row>
+    <row r="31" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="58"/>
       <c r="B31" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-    </row>
-    <row r="32" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A32" s="52"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+    </row>
+    <row r="32" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58"/>
       <c r="B32" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-    </row>
-    <row r="33" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A33" s="52"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="55"/>
+    </row>
+    <row r="33" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="58"/>
       <c r="B33" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-    </row>
-    <row r="34" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A34" s="52"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+    </row>
+    <row r="34" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="58"/>
       <c r="B34" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-    </row>
-    <row r="35" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="53"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+    </row>
+    <row r="35" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="59"/>
       <c r="B35" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-    </row>
-    <row r="36" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="51" t="s">
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+    </row>
+    <row r="36" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="57" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-    </row>
-    <row r="37" spans="1:5" s="17" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A37" s="52"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="55"/>
+    </row>
+    <row r="37" spans="1:5" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="58"/>
       <c r="B37" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-    </row>
-    <row r="38" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A38" s="52"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+    </row>
+    <row r="38" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="58"/>
       <c r="B38" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-    </row>
-    <row r="39" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A39" s="53"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+    </row>
+    <row r="39" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="59"/>
       <c r="B39" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-    </row>
-    <row r="40" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A40" s="51" t="s">
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="57" t="s">
         <v>95</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-    </row>
-    <row r="41" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A41" s="52"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+    </row>
+    <row r="41" spans="1:5" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
       <c r="B41" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-    </row>
-    <row r="42" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A42" s="52"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+    </row>
+    <row r="42" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="58"/>
       <c r="B42" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-    </row>
-    <row r="43" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A43" s="53"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="55"/>
+    </row>
+    <row r="43" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="59"/>
       <c r="B43" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-    </row>
-    <row r="44" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A44" s="51" t="s">
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+    </row>
+    <row r="44" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="57" t="s">
         <v>92</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-    </row>
-    <row r="45" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A45" s="53"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+    </row>
+    <row r="45" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="59"/>
       <c r="B45" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-    </row>
-    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A46" s="62" t="s">
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+    </row>
+    <row r="46" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="61" t="s">
+      <c r="B46" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-    </row>
-    <row r="47" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A47" s="63"/>
-      <c r="B47" s="59" t="s">
+      <c r="C46" s="55"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+    </row>
+    <row r="47" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="61"/>
+      <c r="B47" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-    </row>
-    <row r="48" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A48" s="66"/>
-      <c r="B48" s="60" t="s">
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+    </row>
+    <row r="48" spans="1:5" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="62"/>
+      <c r="B48" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="72"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-    </row>
-    <row r="49" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="70" t="s">
+      <c r="C48" s="55"/>
+      <c r="D48" s="55"/>
+      <c r="E48" s="55"/>
+    </row>
+    <row r="49" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>100</v>
       </c>
       <c r="B49" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-    </row>
-    <row r="50" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="70" t="s">
+      <c r="C49" s="55"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
+    </row>
+    <row r="50" spans="1:5" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B50" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1">
-      <c r="A51" s="70" t="s">
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+    </row>
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B51" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C44:E45"/>
-    <mergeCell ref="C46:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="C4:E6"/>
-    <mergeCell ref="C7:E12"/>
-    <mergeCell ref="C13:E20"/>
-    <mergeCell ref="C21:E29"/>
-    <mergeCell ref="C30:E35"/>
-    <mergeCell ref="C36:E39"/>
-    <mergeCell ref="C40:E43"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A1:B1"/>
@@ -1838,6 +1832,22 @@
     <mergeCell ref="A13:A20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A30:A35"/>
+    <mergeCell ref="C21:E29"/>
+    <mergeCell ref="C30:E35"/>
+    <mergeCell ref="C36:E39"/>
+    <mergeCell ref="C40:E43"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="C4:E6"/>
+    <mergeCell ref="C7:E12"/>
+    <mergeCell ref="C13:E20"/>
+    <mergeCell ref="C44:E45"/>
+    <mergeCell ref="C46:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
@@ -1845,29 +1855,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.5703125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="77.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="77.5703125" style="2"/>
+    <col min="1" max="1" width="68.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="77.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="15">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1878,160 +1888,160 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.75" customHeight="1">
-      <c r="A3" s="51" t="s">
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="57">
+      <c r="B3" s="64">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1">
-      <c r="A4" s="52"/>
-      <c r="B4" s="57"/>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="58"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A5" s="52"/>
-      <c r="B5" s="57"/>
+    <row r="5" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A6" s="52"/>
-      <c r="B6" s="57"/>
+    <row r="6" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="58"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A7" s="52"/>
-      <c r="B7" s="57"/>
+    <row r="7" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="58"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A8" s="52"/>
-      <c r="B8" s="57"/>
+    <row r="8" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="11.25" customHeight="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="54"/>
+    <row r="9" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="65"/>
       <c r="C9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1">
-      <c r="A10" s="49" t="s">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="58">
+      <c r="B10" s="66">
         <v>2</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1">
-      <c r="A11" s="65"/>
-      <c r="B11" s="58"/>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="68"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="A12" s="65"/>
-      <c r="B12" s="58"/>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="68"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="58"/>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="68"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A14" s="65"/>
-      <c r="B14" s="58"/>
+    <row r="14" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="68"/>
+      <c r="B14" s="66"/>
       <c r="C14" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A15" s="50"/>
-      <c r="B15" s="58"/>
+    <row r="15" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="69"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A16" s="48" t="s">
+    <row r="16" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="57">
+      <c r="B16" s="64">
         <v>3</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="57"/>
+    <row r="17" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="70"/>
+      <c r="B17" s="64"/>
       <c r="C17" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A18" s="48"/>
-      <c r="B18" s="57"/>
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="70"/>
+      <c r="B18" s="64"/>
       <c r="C18" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A19" s="48"/>
-      <c r="B19" s="57"/>
+    <row r="19" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="70"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A20" s="48"/>
-      <c r="B20" s="57"/>
+    <row r="20" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="70"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A21" s="48"/>
-      <c r="B21" s="57"/>
+    <row r="21" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="70"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="11" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:B9"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="A3:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.24" right="0.34" top="0.17" bottom="0.21" header="0.17" footer="0.18"/>
   <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
@@ -2039,29 +2049,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A3" activeCellId="1" sqref="C3:C50 A3:A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.5703125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="77.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="6" customWidth="1"/>
-    <col min="4" max="16384" width="77.5703125" style="2"/>
+    <col min="1" max="1" width="68.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="77.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="15">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2072,374 +2082,374 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="51" t="s">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="65">
         <v>1</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A4" s="52"/>
-      <c r="B4" s="56"/>
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="58"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="55"/>
+    <row r="5" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="59"/>
+      <c r="B5" s="72"/>
       <c r="C5" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="65">
         <v>2</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A7" s="52"/>
-      <c r="B7" s="56"/>
+    <row r="7" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="58"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A8" s="52"/>
-      <c r="B8" s="56"/>
+    <row r="8" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="58"/>
+      <c r="B8" s="71"/>
       <c r="C8" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A9" s="52"/>
-      <c r="B9" s="56"/>
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="58"/>
+      <c r="B9" s="71"/>
       <c r="C9" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="52"/>
-      <c r="B10" s="56"/>
+    <row r="10" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="58"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="55"/>
+    <row r="11" spans="1:4" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="59"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="11.25" customHeight="1">
-      <c r="A12" s="52" t="s">
+    <row r="12" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="56">
+      <c r="B12" s="71">
         <v>3</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="11.25" customHeight="1">
-      <c r="A13" s="52"/>
-      <c r="B13" s="56"/>
+    <row r="13" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="64"/>
-    </row>
-    <row r="14" spans="1:4" ht="11.25" customHeight="1">
-      <c r="A14" s="52"/>
-      <c r="B14" s="56"/>
+      <c r="D13" s="25"/>
+    </row>
+    <row r="14" spans="1:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="16" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="52"/>
-      <c r="B15" s="56"/>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="64"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
-      <c r="A16" s="52"/>
-      <c r="B16" s="56"/>
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="64"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1">
-      <c r="A17" s="52"/>
-      <c r="B17" s="56"/>
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="64"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1">
-      <c r="A18" s="52"/>
-      <c r="B18" s="56"/>
+      <c r="D17" s="25"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
+      <c r="B18" s="71"/>
       <c r="C18" s="16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1">
-      <c r="A19" s="53"/>
-      <c r="B19" s="55"/>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1">
-      <c r="A20" s="51" t="s">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="54">
+      <c r="B20" s="65">
         <v>4</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A21" s="52"/>
-      <c r="B21" s="56"/>
+    <row r="21" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A22" s="52"/>
-      <c r="B22" s="56"/>
+    <row r="22" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A23" s="52"/>
-      <c r="B23" s="56"/>
+    <row r="23" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A24" s="52"/>
-      <c r="B24" s="56"/>
+    <row r="24" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="71"/>
       <c r="C24" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A25" s="52"/>
-      <c r="B25" s="56"/>
+    <row r="25" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="71"/>
       <c r="C25" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A26" s="52"/>
-      <c r="B26" s="56"/>
+    <row r="26" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="71"/>
       <c r="C26" s="16" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A27" s="52"/>
-      <c r="B27" s="56"/>
+    <row r="27" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="58"/>
+      <c r="B27" s="71"/>
       <c r="C27" s="16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A28" s="53"/>
-      <c r="B28" s="55"/>
+    <row r="28" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A29" s="51" t="s">
+    <row r="29" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="54">
+      <c r="B29" s="65">
         <v>5</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A30" s="52"/>
-      <c r="B30" s="56"/>
+    <row r="30" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="58"/>
+      <c r="B30" s="71"/>
       <c r="C30" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A31" s="52"/>
-      <c r="B31" s="56"/>
+    <row r="31" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="58"/>
+      <c r="B31" s="71"/>
       <c r="C31" s="16" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A32" s="52"/>
-      <c r="B32" s="56"/>
+    <row r="32" spans="1:4" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="58"/>
+      <c r="B32" s="71"/>
       <c r="C32" s="16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A33" s="52"/>
-      <c r="B33" s="56"/>
+    <row r="33" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="58"/>
+      <c r="B33" s="71"/>
       <c r="C33" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A34" s="53"/>
-      <c r="B34" s="55"/>
+    <row r="34" spans="1:3" s="5" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="72"/>
       <c r="C34" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1">
-      <c r="A35" s="51" t="s">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="54">
+      <c r="B35" s="65">
         <v>6</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1">
-      <c r="A36" s="52"/>
-      <c r="B36" s="56"/>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="58"/>
+      <c r="B36" s="71"/>
       <c r="C36" s="16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1">
-      <c r="A37" s="52"/>
-      <c r="B37" s="56"/>
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="58"/>
+      <c r="B37" s="71"/>
       <c r="C37" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" customHeight="1">
-      <c r="A38" s="53"/>
-      <c r="B38" s="55"/>
+    <row r="38" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
+      <c r="B38" s="72"/>
       <c r="C38" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" customHeight="1">
-      <c r="A39" s="51" t="s">
+    <row r="39" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="54">
+      <c r="B39" s="65">
         <v>7</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1">
-      <c r="A40" s="52"/>
-      <c r="B40" s="56"/>
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="58"/>
+      <c r="B40" s="71"/>
       <c r="C40" s="16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1">
-      <c r="A41" s="52"/>
-      <c r="B41" s="56"/>
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="58"/>
+      <c r="B41" s="71"/>
       <c r="C41" s="16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1">
-      <c r="A42" s="53"/>
-      <c r="B42" s="55"/>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="59"/>
+      <c r="B42" s="72"/>
       <c r="C42" s="11" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1">
-      <c r="A43" s="51" t="s">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="54">
+      <c r="B43" s="65">
         <v>8</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1">
-      <c r="A44" s="53"/>
-      <c r="B44" s="55"/>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="59"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1">
-      <c r="A45" s="62" t="s">
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="54">
+      <c r="B45" s="65">
         <v>9</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="24" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1">
-      <c r="A46" s="63"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="59" t="s">
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="61"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1">
-      <c r="A47" s="66"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="60" t="s">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="62"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1">
-      <c r="A48" s="67" t="s">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="68">
+      <c r="B48" s="27">
         <v>10</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1">
-      <c r="A49" s="67" t="s">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
         <v>102</v>
       </c>
       <c r="B49" s="20">
@@ -2449,8 +2459,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15">
-      <c r="A50" s="67" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="26" t="s">
         <v>105</v>
       </c>
       <c r="B50" s="21">
@@ -2462,23 +2472,23 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="A20:A28"/>
     <mergeCell ref="A45:A47"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B20:B28"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A29:A34"/>
     <mergeCell ref="B35:B38"/>
     <mergeCell ref="B45:B47"/>
   </mergeCells>

</xml_diff>